<commit_message>
Machine Learning implementet, GUI
</commit_message>
<xml_diff>
--- a/Trainingsdaten.xlsx
+++ b/Trainingsdaten.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neugebauer\Desktop\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\source\repos\FindMyID\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50E4DB9-6199-4E0C-81AB-EC38B5FAA1DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trainingsdaten" sheetId="1" r:id="rId1"/>
@@ -19,57 +20,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t>Wie besprochen bearbeiten wir aktuell den Auftrag A0123456. Hierbei müssen wichtige Tätigkeiten erledigt werden. Wir haben bereits im Auftrag A0647386 ähnliche Tätigkeiten erledigt.</t>
-  </si>
-  <si>
-    <t>A0123456</t>
-  </si>
-  <si>
-    <t>Bezogen auf Auftrag A0529384 haben wir ein Problem. Wir können die rechtzeitige fertigstellung nicht mehr garantieren da wir durch den Auftrag A0845287 aufgehalten werden.</t>
-  </si>
-  <si>
-    <t>A0529384</t>
-  </si>
-  <si>
-    <t>Ich hoffe gestern hat mit dem Auftrag A0392876 alles geklappt. Ich melde mich wegen Auftrag A0638276. Alles läuft super und sollte bald fertiggestellt sein</t>
-  </si>
-  <si>
-    <t>A0638276</t>
-  </si>
-  <si>
-    <t>Es geht um A0637465. Wir schaffen das so nicht und benötigen bessere Unterstützung. Bei A0427487 hat es doch auch geklappt.</t>
-  </si>
-  <si>
-    <t>A0637465</t>
-  </si>
-  <si>
-    <t>A0938291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich melde mich bezüglich A0938291 hat alles geklappt. Mit A0382956 stimmt etwas nicht.	</t>
-  </si>
-  <si>
-    <t>Es geht um Auftrag A0123456.</t>
-  </si>
-  <si>
-    <t>Wegen Auftrag A0123456. Alles passt. Auftrag war nicht so gut.</t>
-  </si>
-  <si>
-    <t>Ich finde den Prozess im Auftrag A0123456 gut.</t>
-  </si>
-  <si>
-    <t>Ich melde mich wegen Auftrag A0123456.</t>
-  </si>
-  <si>
-    <t>Ich schreibe wegen Auftrag A0123456.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Wie besprochen bearbeiten wir aktuell den Auftrag A0000001. Hierbei müssen wichtige Tätigkeiten erledigt werden. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezogen auf Auftrag A0000002 haben wir ein Problem. </t>
+  </si>
+  <si>
+    <t>Ich melde mich wegen Auftrag A0000003. Alles läuft super und sollte bald fertiggestellt sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es geht um A0000004. Wir schaffen das so nicht und benötigen bessere Unterstützung. </t>
+  </si>
+  <si>
+    <t>Ich melde mich bezüglich A0000005 hat alles geklappt.</t>
+  </si>
+  <si>
+    <t>Ich melde mich wegen Auftrag A0000006.</t>
+  </si>
+  <si>
+    <t>Ich finde den Prozess im Auftrag A0000007 gut.</t>
+  </si>
+  <si>
+    <t>Wegen Auftrag A0000008. Alles passt.</t>
+  </si>
+  <si>
+    <t>Es geht um Auftrag A0000009.</t>
+  </si>
+  <si>
+    <t>Ich schreibe wegen Auftrag A0000010.</t>
+  </si>
+  <si>
+    <t>Bezüglich Auftrag A0000011.</t>
+  </si>
+  <si>
+    <t>Nochmal wegen Auftrag A0000012.</t>
+  </si>
+  <si>
+    <t>Ich melde mich wegen dem Auftrag A0000013.</t>
+  </si>
+  <si>
+    <t>Ich melde mich wegen des Auftrages A0000014.</t>
+  </si>
+  <si>
+    <t>Wegen dem Auftarg A0000015.</t>
+  </si>
+  <si>
+    <t>Wir haben bereits im Auftrag A0000016 ähnliche Tätigkeiten erledigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mit A0000017 stimmt etwas nicht.</t>
+  </si>
+  <si>
+    <t>Bei A0000018 hat es doch auch geklappt.</t>
+  </si>
+  <si>
+    <t>Ich hoffe gestern hat mit dem Auftrag A0000019 alles geklappt.</t>
+  </si>
+  <si>
+    <t>Wir können die rechtzeitige fertigstellung nicht mehr garantieren da wir durch den Auftrag A0000020 aufgehalten werden.</t>
+  </si>
+  <si>
+    <t>Hat bei Auftrag A0000021 alles geklappt?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -869,11 +888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,80 +904,168 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>